<commit_message>
New excel file, fixed
</commit_message>
<xml_diff>
--- a/ABBREV-abbreviated.xlsx
+++ b/ABBREV-abbreviated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\poster-gui\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D24B2ECC-47A3-40A3-A8E1-71E5E408C2B5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D2727D71-951A-44A9-BC71-9E6A6B09F25A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" xr2:uid="{87936AB8-C06E-4E0B-9AB2-E3580F47D6CA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="120">
   <si>
     <t>01001</t>
   </si>
@@ -349,13 +349,49 @@
   </si>
   <si>
     <t>1 fish</t>
+  </si>
+  <si>
+    <t>NDB_No</t>
+  </si>
+  <si>
+    <t>Shrt_Desc</t>
+  </si>
+  <si>
+    <t>Water_(g)</t>
+  </si>
+  <si>
+    <t>Energ_Kcal</t>
+  </si>
+  <si>
+    <t>Protein_(g)</t>
+  </si>
+  <si>
+    <t>Lipid_Tot_(g)</t>
+  </si>
+  <si>
+    <t>Carbohydrt_(g)</t>
+  </si>
+  <si>
+    <t>Sugar_Tot_(g)</t>
+  </si>
+  <si>
+    <t>Calcium_(mg)</t>
+  </si>
+  <si>
+    <t>Iron_(mg)</t>
+  </si>
+  <si>
+    <t>Sodium_(mg)</t>
+  </si>
+  <si>
+    <t>GmWt_Desc1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -368,16 +404,28 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -400,17 +448,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -726,257 +792,255 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EEB7256-A5BE-4515-8B36-EAC2FE228CF1}">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C2" s="2">
         <v>15.87</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D2" s="2">
         <v>717</v>
       </c>
-      <c r="E1" s="2">
+      <c r="E2" s="2">
         <v>0.85</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F2" s="2">
         <v>81.11</v>
       </c>
-      <c r="G1" s="2">
+      <c r="G2" s="2">
         <v>0.06</v>
       </c>
-      <c r="H1" s="2">
+      <c r="H2" s="2">
         <v>0.06</v>
       </c>
-      <c r="I1" s="2">
+      <c r="I2" s="2">
         <v>24</v>
       </c>
-      <c r="J1" s="2">
+      <c r="J2" s="2">
         <v>0.02</v>
       </c>
-      <c r="K1" s="2">
+      <c r="K2" s="2">
         <v>643</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2">
-        <v>50.01</v>
-      </c>
-      <c r="D2" s="2">
-        <v>300</v>
-      </c>
-      <c r="E2" s="2">
-        <v>22.17</v>
-      </c>
-      <c r="F2" s="2">
-        <v>22.35</v>
-      </c>
-      <c r="G2" s="2">
-        <v>2.19</v>
-      </c>
-      <c r="H2" s="2">
-        <v>1.03</v>
-      </c>
-      <c r="I2" s="2">
-        <v>505</v>
-      </c>
-      <c r="J2" s="2">
-        <v>0.44</v>
-      </c>
-      <c r="K2" s="2">
-        <v>627</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2">
+        <v>50.01</v>
+      </c>
+      <c r="D3" s="2">
+        <v>300</v>
+      </c>
+      <c r="E3" s="2">
+        <v>22.17</v>
+      </c>
+      <c r="F3" s="2">
+        <v>22.35</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2.19</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1.03</v>
+      </c>
+      <c r="I3" s="2">
+        <v>505</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.44</v>
+      </c>
+      <c r="K3" s="2">
+        <v>627</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C4" s="2">
         <v>87.69</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D4" s="2">
         <v>64</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E4" s="2">
         <v>3.28</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F4" s="2">
         <v>3.66</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G4" s="2">
         <v>4.6500000000000004</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I4" s="2">
         <v>119</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J4" s="2">
         <v>0.05</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K4" s="2">
         <v>49</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:12" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C5" s="2">
         <v>79</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D5" s="2">
         <v>85</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E5" s="2">
         <v>4.93</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F5" s="2">
         <v>1.25</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G5" s="2">
         <v>13.8</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H5" s="2">
         <v>13.8</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I5" s="2">
         <v>171</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J5" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K5" s="2">
         <v>66</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:12" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C6" s="2">
         <v>76.150000000000006</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D6" s="2">
         <v>143</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E6" s="2">
         <v>12.56</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F6" s="2">
         <v>9.51</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G6" s="2">
         <v>0.72</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H6" s="2">
         <v>0.37</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I6" s="2">
         <v>56</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J6" s="2">
         <v>1.75</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K6" s="2">
         <v>142</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="2">
-        <v>59.45</v>
-      </c>
-      <c r="D6" s="2">
-        <v>239</v>
-      </c>
-      <c r="E6" s="2">
-        <v>27.3</v>
-      </c>
-      <c r="F6" s="2">
-        <v>13.6</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2">
-        <v>15</v>
-      </c>
-      <c r="J6" s="2">
-        <v>1.26</v>
-      </c>
-      <c r="K6" s="2">
-        <v>82</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2">
-        <v>62.07</v>
+        <v>59.45</v>
       </c>
       <c r="D7" s="2">
-        <v>203</v>
+        <v>239</v>
       </c>
       <c r="E7" s="2">
-        <v>27.37</v>
+        <v>27.3</v>
       </c>
       <c r="F7" s="2">
-        <v>10.4</v>
+        <v>13.6</v>
       </c>
       <c r="G7" s="2">
         <v>0</v>
@@ -985,390 +1049,390 @@
         <v>0</v>
       </c>
       <c r="I7" s="2">
+        <v>15</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1.26</v>
+      </c>
+      <c r="K7" s="2">
+        <v>82</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2">
+        <v>62.07</v>
+      </c>
+      <c r="D8" s="2">
+        <v>203</v>
+      </c>
+      <c r="E8" s="2">
+        <v>27.37</v>
+      </c>
+      <c r="F8" s="2">
+        <v>10.4</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
         <v>28</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J8" s="2">
         <v>1.52</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K8" s="2">
         <v>78</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="2">
-        <v>88.8</v>
-      </c>
-      <c r="D8" s="2">
-        <v>46</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1.59</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1.19</v>
-      </c>
-      <c r="G8" s="2">
-        <v>7.19</v>
-      </c>
-      <c r="H8" s="2">
-        <v>0.79</v>
-      </c>
-      <c r="I8" s="2">
-        <v>0</v>
-      </c>
-      <c r="J8" s="2">
-        <v>0</v>
-      </c>
-      <c r="K8" s="2">
-        <v>325</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2">
+        <v>88.8</v>
+      </c>
+      <c r="D9" s="2">
+        <v>46</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.59</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1.19</v>
+      </c>
+      <c r="G9" s="2">
+        <v>7.19</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.79</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>325</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C10" s="2">
         <v>7.37</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D10" s="2">
         <v>369</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E10" s="2">
         <v>10.39</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F10" s="2">
         <v>5.0999999999999996</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G10" s="2">
         <v>74.52</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H10" s="2">
         <v>21.14</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I10" s="2">
         <v>229</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J10" s="2">
         <v>8.31</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K10" s="2">
         <v>416</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:12" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C11" s="2">
         <v>9.69</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D11" s="2">
         <v>365</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E11" s="2">
         <v>10.48</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F11" s="2">
         <v>0.49</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G11" s="2">
         <v>77.2</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H11" s="2">
         <v>0.7</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I11" s="2">
         <v>377</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J11" s="2">
         <v>40.93</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K11" s="2">
         <v>3</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:12" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C12" s="2">
         <v>85.97</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D12" s="2">
         <v>49</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E12" s="2">
         <v>0.91</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F12" s="2">
         <v>0.15</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G12" s="2">
         <v>12.54</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H12" s="2">
         <v>8.5</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I12" s="2">
         <v>43</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J12" s="2">
         <v>0.13</v>
-      </c>
-      <c r="K11" s="2">
-        <v>1</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="2">
-        <v>86</v>
-      </c>
-      <c r="D12" s="2">
-        <v>50</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0.54</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="G12" s="2">
-        <v>13.12</v>
-      </c>
-      <c r="H12" s="2">
-        <v>9.85</v>
-      </c>
-      <c r="I12" s="2">
-        <v>13</v>
-      </c>
-      <c r="J12" s="2">
-        <v>0.28999999999999998</v>
       </c>
       <c r="K12" s="2">
         <v>1</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C13" s="2">
-        <v>78.05</v>
+        <v>86</v>
       </c>
       <c r="D13" s="2">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="E13" s="2">
-        <v>0.52</v>
+        <v>0.54</v>
       </c>
       <c r="F13" s="2">
-        <v>0.14000000000000001</v>
+        <v>0.12</v>
       </c>
       <c r="G13" s="2">
-        <v>21</v>
+        <v>13.12</v>
       </c>
       <c r="H13" s="2">
-        <v>18.61</v>
+        <v>9.85</v>
       </c>
       <c r="I13" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="J13" s="2">
-        <v>0.47</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="K13" s="2">
         <v>1</v>
       </c>
       <c r="L13" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="2">
+        <v>78.05</v>
+      </c>
+      <c r="D14" s="2">
+        <v>78</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G14" s="2">
+        <v>21</v>
+      </c>
+      <c r="H14" s="2">
+        <v>18.61</v>
+      </c>
+      <c r="I14" s="2">
+        <v>11</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1</v>
+      </c>
+      <c r="L14" s="1" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="2">
-        <v>67.67</v>
-      </c>
-      <c r="D14" s="2">
-        <v>145</v>
-      </c>
-      <c r="E14" s="2">
-        <v>20.93</v>
-      </c>
-      <c r="F14" s="2">
-        <v>5.53</v>
-      </c>
-      <c r="G14" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="H14" s="2">
-        <v>0</v>
-      </c>
-      <c r="I14" s="2">
-        <v>8</v>
-      </c>
-      <c r="J14" s="2">
-        <v>1.48</v>
-      </c>
-      <c r="K14" s="2">
-        <v>1203</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="2">
+        <v>67.67</v>
+      </c>
+      <c r="D15" s="2">
+        <v>145</v>
+      </c>
+      <c r="E15" s="2">
+        <v>20.93</v>
+      </c>
+      <c r="F15" s="2">
+        <v>5.53</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2">
+        <v>8</v>
+      </c>
+      <c r="J15" s="2">
+        <v>1.48</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1203</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C16" s="2">
         <v>58.01</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D16" s="2">
         <v>162</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E16" s="2">
         <v>9.31</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F16" s="2">
         <v>0.48</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G16" s="2">
         <v>30.87</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I16" s="2">
         <v>52</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J16" s="2">
         <v>2.71</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K16" s="2">
         <v>83</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="2">
-        <v>89.3</v>
-      </c>
-      <c r="D16" s="2">
-        <v>34</v>
-      </c>
-      <c r="E16" s="2">
-        <v>2.82</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0.37</v>
-      </c>
-      <c r="G16" s="2">
-        <v>6.64</v>
-      </c>
-      <c r="H16" s="2">
-        <v>1.7</v>
-      </c>
-      <c r="I16" s="2">
-        <v>47</v>
-      </c>
-      <c r="J16" s="2">
-        <v>0.73</v>
-      </c>
-      <c r="K16" s="2">
-        <v>33</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="2">
+        <v>89.3</v>
+      </c>
+      <c r="D17" s="2">
+        <v>34</v>
+      </c>
+      <c r="E17" s="2">
+        <v>2.82</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.37</v>
+      </c>
+      <c r="G17" s="2">
+        <v>6.64</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="I17" s="2">
         <v>47</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="2">
-        <v>92.18</v>
-      </c>
-      <c r="D17" s="2">
-        <v>25</v>
-      </c>
-      <c r="E17" s="2">
-        <v>1.28</v>
-      </c>
-      <c r="F17" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="G17" s="2">
-        <v>5.8</v>
-      </c>
-      <c r="H17" s="2">
-        <v>3.2</v>
-      </c>
-      <c r="I17" s="2">
-        <v>40</v>
-      </c>
       <c r="J17" s="2">
-        <v>0.47</v>
+        <v>0.73</v>
       </c>
       <c r="K17" s="2">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>46</v>
@@ -1376,563 +1440,563 @@
     </row>
     <row r="18" spans="1:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C18" s="2">
-        <v>88.29</v>
+        <v>92.18</v>
       </c>
       <c r="D18" s="2">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="E18" s="2">
-        <v>0.93</v>
+        <v>1.28</v>
       </c>
       <c r="F18" s="2">
-        <v>0.24</v>
+        <v>0.1</v>
       </c>
       <c r="G18" s="2">
-        <v>9.58</v>
+        <v>5.8</v>
       </c>
       <c r="H18" s="2">
-        <v>4.74</v>
+        <v>3.2</v>
       </c>
       <c r="I18" s="2">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="J18" s="2">
-        <v>0.3</v>
+        <v>0.47</v>
       </c>
       <c r="K18" s="2">
-        <v>69</v>
+        <v>18</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="2">
+        <v>88.29</v>
+      </c>
+      <c r="D19" s="2">
+        <v>41</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.93</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="G19" s="2">
+        <v>9.58</v>
+      </c>
+      <c r="H19" s="2">
+        <v>4.74</v>
+      </c>
+      <c r="I19" s="2">
+        <v>33</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="K19" s="2">
+        <v>69</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C20" s="2">
         <v>95.63</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D20" s="2">
         <v>13</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E20" s="2">
         <v>1.35</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F20" s="2">
         <v>0.22</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G20" s="2">
         <v>2.23</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H20" s="2">
         <v>0.94</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I20" s="2">
         <v>35</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J20" s="2">
         <v>1.24</v>
       </c>
-      <c r="K19" s="2">
+      <c r="K20" s="2">
         <v>5</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:12" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C21" s="2">
         <v>92.82</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D21" s="2">
         <v>22</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E21" s="2">
         <v>2.11</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F21" s="2">
         <v>0.35</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G21" s="2">
         <v>3.87</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H21" s="2">
         <v>2.5</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I21" s="2">
         <v>3</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J21" s="2">
         <v>0.31</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K21" s="2">
         <v>9</v>
       </c>
-      <c r="L20" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C22" s="2">
         <v>89.11</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D22" s="2">
         <v>40</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E22" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F22" s="2">
         <v>0.1</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G22" s="2">
         <v>9.34</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H22" s="2">
         <v>4.24</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I22" s="2">
         <v>23</v>
       </c>
-      <c r="J21" s="2">
+      <c r="J22" s="2">
         <v>0.21</v>
       </c>
-      <c r="K21" s="2">
+      <c r="K22" s="2">
         <v>4</v>
       </c>
-      <c r="L21" s="1" t="s">
+      <c r="L22" s="1" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="2">
-        <v>79.25</v>
-      </c>
-      <c r="D22" s="2">
-        <v>77</v>
-      </c>
-      <c r="E22" s="2">
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="F22" s="2">
-        <v>0.09</v>
-      </c>
-      <c r="G22" s="2">
-        <v>17.489999999999998</v>
-      </c>
-      <c r="H22" s="2">
-        <v>0.82</v>
-      </c>
-      <c r="I22" s="2">
-        <v>12</v>
-      </c>
-      <c r="J22" s="2">
-        <v>0.81</v>
-      </c>
-      <c r="K22" s="2">
-        <v>6</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C23" s="2">
-        <v>94.24</v>
+        <v>79.25</v>
       </c>
       <c r="D23" s="2">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="E23" s="2">
-        <v>0.85</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="F23" s="2">
-        <v>0.28999999999999998</v>
+        <v>0.09</v>
       </c>
       <c r="G23" s="2">
-        <v>3.53</v>
+        <v>17.489999999999998</v>
       </c>
       <c r="H23" s="2">
-        <v>2.58</v>
+        <v>0.82</v>
       </c>
       <c r="I23" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J23" s="2">
-        <v>0.39</v>
+        <v>0.81</v>
       </c>
       <c r="K23" s="2">
-        <v>253</v>
+        <v>6</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="2">
+        <v>94.24</v>
+      </c>
+      <c r="D24" s="2">
+        <v>17</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G24" s="2">
+        <v>3.53</v>
+      </c>
+      <c r="H24" s="2">
+        <v>2.58</v>
+      </c>
+      <c r="I24" s="2">
+        <v>10</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0.39</v>
+      </c>
+      <c r="K24" s="2">
+        <v>253</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C25" s="2">
         <v>5.31</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D25" s="2">
         <v>628</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E25" s="2">
         <v>14.95</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F25" s="2">
         <v>60.75</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G25" s="2">
         <v>16.7</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H25" s="2">
         <v>4.34</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I25" s="2">
         <v>114</v>
       </c>
-      <c r="J24" s="2">
+      <c r="J25" s="2">
         <v>4.7</v>
       </c>
-      <c r="K24" s="2">
+      <c r="K25" s="2">
         <v>0</v>
       </c>
-      <c r="L24" s="1" t="s">
+      <c r="L25" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:12" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C26" s="2">
         <v>53.39</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D26" s="2">
         <v>280</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E26" s="2">
         <v>28.97</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F26" s="2">
         <v>17.37</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G26" s="2">
         <v>0</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H26" s="2">
         <v>0</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I26" s="2">
         <v>17</v>
       </c>
-      <c r="J25" s="2">
+      <c r="J26" s="2">
         <v>2.4</v>
       </c>
-      <c r="K25" s="2">
+      <c r="K26" s="2">
         <v>49</v>
       </c>
-      <c r="L25" s="1" t="s">
+      <c r="L26" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:12" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C27" s="2">
         <v>89.28</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D27" s="2">
         <v>47</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E27" s="2">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F27" s="2">
         <v>0.97</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G27" s="2">
         <v>9.17</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H27" s="2">
         <v>5.28</v>
       </c>
-      <c r="I26" s="2">
+      <c r="I27" s="2">
         <v>118</v>
       </c>
-      <c r="J26" s="2">
+      <c r="J27" s="2">
         <v>0.2</v>
       </c>
-      <c r="K26" s="2">
+      <c r="K27" s="2">
         <v>39</v>
       </c>
-      <c r="L26" s="1" t="s">
+      <c r="L27" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C28" s="2">
         <v>81.22</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D28" s="2">
         <v>82</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E28" s="2">
         <v>17.809999999999999</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F28" s="2">
         <v>0.67</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G28" s="2">
         <v>0</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H28" s="2">
         <v>0</v>
       </c>
-      <c r="I27" s="2">
+      <c r="I28" s="2">
         <v>16</v>
       </c>
-      <c r="J27" s="2">
+      <c r="J28" s="2">
         <v>0.38</v>
       </c>
-      <c r="K27" s="2">
+      <c r="K28" s="2">
         <v>54</v>
       </c>
-      <c r="L27" s="1" t="s">
+      <c r="L28" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="1" t="s">
+    <row r="29" spans="1:12" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C29" s="2">
         <v>66.59</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D29" s="2">
         <v>166</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E29" s="2">
         <v>7.9</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F29" s="2">
         <v>9.6</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G29" s="2">
         <v>14.29</v>
       </c>
-      <c r="I28" s="2">
+      <c r="I29" s="2">
         <v>38</v>
       </c>
-      <c r="J28" s="2">
+      <c r="J29" s="2">
         <v>2.44</v>
       </c>
-      <c r="K28" s="2">
+      <c r="K29" s="2">
         <v>379</v>
       </c>
-      <c r="L28" s="1" t="s">
+      <c r="L29" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="1" t="s">
+    <row r="30" spans="1:12" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C30" s="2">
         <v>82.31</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D30" s="2">
         <v>83</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E30" s="2">
         <v>9.98</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F30" s="2">
         <v>5.26</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G30" s="2">
         <v>1.18</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H30" s="2">
         <v>0.71</v>
       </c>
-      <c r="I29" s="2">
+      <c r="I30" s="2">
         <v>282</v>
       </c>
-      <c r="J29" s="2">
+      <c r="J30" s="2">
         <v>2.04</v>
       </c>
-      <c r="K29" s="2">
+      <c r="K30" s="2">
         <v>4</v>
       </c>
-      <c r="L29" s="1" t="s">
+      <c r="L30" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="1" t="s">
+    <row r="31" spans="1:12" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C31" s="2">
         <v>69.64</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D31" s="2">
         <v>114</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E31" s="2">
         <v>9.02</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F31" s="2">
         <v>0.38</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G31" s="2">
         <v>19.54</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H31" s="2">
         <v>1.8</v>
       </c>
-      <c r="I30" s="2">
+      <c r="I31" s="2">
         <v>19</v>
       </c>
-      <c r="J30" s="2">
+      <c r="J31" s="2">
         <v>3.33</v>
       </c>
-      <c r="K30" s="2">
+      <c r="K31" s="2">
         <v>238</v>
       </c>
-      <c r="L30" s="1" t="s">
+      <c r="L31" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="115.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="1" t="s">
+    <row r="32" spans="1:12" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C32" s="2">
         <v>73.680000000000007</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D32" s="2">
         <v>138</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E32" s="2">
         <v>20.48</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F32" s="2">
         <v>5.64</v>
       </c>
-      <c r="G31" s="2">
+      <c r="G32" s="2">
         <v>0</v>
       </c>
-      <c r="I31" s="2">
+      <c r="I32" s="2">
         <v>10</v>
       </c>
-      <c r="J31" s="2">
+      <c r="J32" s="2">
         <v>1.75</v>
       </c>
-      <c r="K31" s="2">
+      <c r="K32" s="2">
         <v>80</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C32" s="2">
-        <v>13.6</v>
-      </c>
-      <c r="D32" s="2">
-        <v>405</v>
-      </c>
-      <c r="E32" s="2">
-        <v>4.8</v>
-      </c>
-      <c r="F32" s="2">
-        <v>16.3</v>
-      </c>
-      <c r="G32" s="2">
-        <v>63.9</v>
-      </c>
-      <c r="H32" s="2">
-        <v>36.61</v>
-      </c>
-      <c r="I32" s="2">
-        <v>29</v>
-      </c>
-      <c r="J32" s="2">
-        <v>2.25</v>
-      </c>
-      <c r="K32" s="2">
-        <v>286</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>84</v>
@@ -1940,285 +2004,285 @@
     </row>
     <row r="33" spans="1:12" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="2">
+        <v>13.6</v>
+      </c>
+      <c r="D33" s="2">
+        <v>405</v>
+      </c>
+      <c r="E33" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F33" s="2">
+        <v>16.3</v>
+      </c>
+      <c r="G33" s="2">
+        <v>63.9</v>
+      </c>
+      <c r="H33" s="2">
+        <v>36.61</v>
+      </c>
+      <c r="I33" s="2">
+        <v>29</v>
+      </c>
+      <c r="J33" s="2">
+        <v>2.25</v>
+      </c>
+      <c r="K33" s="2">
+        <v>286</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C34" s="2">
         <v>33.1</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D34" s="2">
         <v>266</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E34" s="2">
         <v>8.6999999999999993</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F34" s="2">
         <v>4.7</v>
       </c>
-      <c r="G33" s="2">
+      <c r="G34" s="2">
         <v>51.1</v>
       </c>
-      <c r="H33" s="2">
+      <c r="H34" s="2">
         <v>8.4600000000000009</v>
       </c>
-      <c r="I33" s="2">
+      <c r="I34" s="2">
         <v>106</v>
       </c>
-      <c r="J33" s="2">
+      <c r="J34" s="2">
         <v>2.42</v>
       </c>
-      <c r="K33" s="2">
+      <c r="K34" s="2">
         <v>521</v>
       </c>
-      <c r="L33" s="1" t="s">
+      <c r="L34" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:12" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C35" s="2">
         <v>39.6</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D35" s="2">
         <v>238</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E35" s="2">
         <v>10.66</v>
-      </c>
-      <c r="F34" s="2">
-        <v>2.15</v>
-      </c>
-      <c r="G34" s="2">
-        <v>43.91</v>
-      </c>
-      <c r="H34" s="2">
-        <v>5</v>
-      </c>
-      <c r="I34" s="2">
-        <v>684</v>
-      </c>
-      <c r="J34" s="2">
-        <v>4.8899999999999997</v>
-      </c>
-      <c r="K34" s="2">
-        <v>478</v>
-      </c>
-      <c r="L34" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C35" s="2">
-        <v>75.150000000000006</v>
-      </c>
-      <c r="D35" s="2">
-        <v>108</v>
-      </c>
-      <c r="E35" s="2">
-        <v>3.23</v>
       </c>
       <c r="F35" s="2">
         <v>2.15</v>
       </c>
       <c r="G35" s="2">
+        <v>43.91</v>
+      </c>
+      <c r="H35" s="2">
+        <v>5</v>
+      </c>
+      <c r="I35" s="2">
+        <v>684</v>
+      </c>
+      <c r="J35" s="2">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="K35" s="2">
+        <v>478</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" s="2">
+        <v>75.150000000000006</v>
+      </c>
+      <c r="D36" s="2">
+        <v>108</v>
+      </c>
+      <c r="E36" s="2">
+        <v>3.23</v>
+      </c>
+      <c r="F36" s="2">
+        <v>2.15</v>
+      </c>
+      <c r="G36" s="2">
         <v>18.39</v>
       </c>
-      <c r="H35" s="2">
+      <c r="H36" s="2">
         <v>11.59</v>
       </c>
-      <c r="I35" s="2">
+      <c r="I36" s="2">
         <v>95</v>
       </c>
-      <c r="J35" s="2">
+      <c r="J36" s="2">
         <v>0.11</v>
       </c>
-      <c r="K35" s="2">
+      <c r="K36" s="2">
         <v>97</v>
       </c>
-      <c r="L35" s="1" t="s">
+      <c r="L36" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:12" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C37" s="2">
         <v>12.37</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D37" s="2">
         <v>362</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E37" s="2">
         <v>7.5</v>
       </c>
-      <c r="F36" s="2">
+      <c r="F37" s="2">
         <v>2.68</v>
       </c>
-      <c r="G36" s="2">
+      <c r="G37" s="2">
         <v>76.17</v>
       </c>
-      <c r="I36" s="2">
+      <c r="I37" s="2">
         <v>33</v>
       </c>
-      <c r="J36" s="2">
+      <c r="J37" s="2">
         <v>1.8</v>
       </c>
-      <c r="K36" s="2">
+      <c r="K37" s="2">
         <v>4</v>
       </c>
-      <c r="L36" s="1" t="s">
+      <c r="L37" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="115.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="1" t="s">
+    <row r="38" spans="1:12" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C38" s="2">
         <v>49.15</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D38" s="2">
         <v>248</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E38" s="2">
         <v>11.34</v>
       </c>
-      <c r="F37" s="2">
+      <c r="F38" s="2">
         <v>10.95</v>
       </c>
-      <c r="G37" s="2">
+      <c r="G38" s="2">
         <v>26.01</v>
       </c>
-      <c r="H37" s="2">
+      <c r="H38" s="2">
         <v>3.04</v>
       </c>
-      <c r="I37" s="2">
+      <c r="I38" s="2">
         <v>104</v>
       </c>
-      <c r="J37" s="2">
+      <c r="J38" s="2">
         <v>1.53</v>
       </c>
-      <c r="K37" s="2">
+      <c r="K38" s="2">
         <v>658</v>
       </c>
-      <c r="L37" s="1" t="s">
+      <c r="L38" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="1" t="s">
+    <row r="39" spans="1:12" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C39" s="2">
         <v>53.37</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D39" s="2">
         <v>214</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E39" s="2">
         <v>5.95</v>
       </c>
-      <c r="F38" s="2">
+      <c r="F39" s="2">
         <v>6.97</v>
       </c>
-      <c r="G38" s="2">
+      <c r="G39" s="2">
         <v>31.77</v>
       </c>
-      <c r="H38" s="2">
+      <c r="H39" s="2">
         <v>5.96</v>
       </c>
-      <c r="I38" s="2">
+      <c r="I39" s="2">
         <v>50</v>
       </c>
-      <c r="J38" s="2">
+      <c r="J39" s="2">
         <v>1.95</v>
       </c>
-      <c r="K38" s="2">
+      <c r="K39" s="2">
         <v>490</v>
       </c>
-      <c r="L38" s="1" t="s">
+      <c r="L39" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="1" t="s">
+    <row r="40" spans="1:12" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C40" s="2">
         <v>69.64</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D40" s="2">
         <v>153</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E40" s="2">
         <v>21.94</v>
       </c>
-      <c r="F39" s="2">
+      <c r="F40" s="2">
         <v>7.28</v>
-      </c>
-      <c r="G39" s="2">
-        <v>0</v>
-      </c>
-      <c r="H39" s="2">
-        <v>0</v>
-      </c>
-      <c r="I39" s="2">
-        <v>7</v>
-      </c>
-      <c r="J39" s="2">
-        <v>0.53</v>
-      </c>
-      <c r="K39" s="2">
-        <v>60</v>
-      </c>
-      <c r="L39" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C40" s="2">
-        <v>78.5</v>
-      </c>
-      <c r="D40" s="2">
-        <v>89</v>
-      </c>
-      <c r="E40" s="2">
-        <v>19.8</v>
-      </c>
-      <c r="F40" s="2">
-        <v>0.5</v>
       </c>
       <c r="G40" s="2">
         <v>0</v>
@@ -2227,15 +2291,53 @@
         <v>0</v>
       </c>
       <c r="I40" s="2">
+        <v>7</v>
+      </c>
+      <c r="J40" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="K40" s="2">
+        <v>60</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" s="2">
+        <v>78.5</v>
+      </c>
+      <c r="D41" s="2">
+        <v>89</v>
+      </c>
+      <c r="E41" s="2">
+        <v>19.8</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G41" s="2">
+        <v>0</v>
+      </c>
+      <c r="H41" s="2">
+        <v>0</v>
+      </c>
+      <c r="I41" s="2">
         <v>118</v>
       </c>
-      <c r="J40" s="2">
+      <c r="J41" s="2">
         <v>1.4</v>
       </c>
-      <c r="K40" s="2">
+      <c r="K41" s="2">
         <v>68</v>
       </c>
-      <c r="L40" s="1" t="s">
+      <c r="L41" s="1" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>